<commit_message>
Fix the excel conflict issue
</commit_message>
<xml_diff>
--- a/NformTester/NformTester/keywordscripts/TST938_ConfigurationOnDevice_properties.xlsx
+++ b/NformTester/NformTester/keywordscripts/TST938_ConfigurationOnDevice_properties.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="15" windowWidth="15480" windowHeight="11640"/>
@@ -1205,6 +1205,7 @@
     <definedName name="PauseCol">'Form DataValDepend'!$CD:$CD</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -4766,7 +4767,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O233"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="H56" sqref="H56"/>
     </sheetView>
   </sheetViews>

</xml_diff>